<commit_message>
Update after data extraction
</commit_message>
<xml_diff>
--- a/cs03_VaVaI_AI/06_Data/data_extraction_sheet.xlsx
+++ b/cs03_VaVaI_AI/06_Data/data_extraction_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\GitHub\data-analyst-portfolio-project-2022\cs03_VaVaI_AI\06_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40A4813-9D8B-4A1E-9A42-1C66F646343C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581A3E67-BDCB-4DAA-948C-90D18C610E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7545" yWindow="3585" windowWidth="25275" windowHeight="16815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -181,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -193,7 +193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -205,7 +205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -217,7 +217,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -229,7 +229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -241,7 +241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -258,7 +258,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="118">
   <si>
     <t>your comment</t>
   </si>
@@ -324,9 +324,6 @@
 </t>
   </si>
   <si>
-    <t>row created by CADIMA</t>
-  </si>
-  <si>
     <t>Jimenez-Bravo, DM; Murciego, AL; Mendes, AS; San Blas, HS; Bajo, J</t>
   </si>
   <si>
@@ -454,6 +451,180 @@
   </si>
   <si>
     <t>https://1drv.ms/b/s!AikiH0T16G7Y9Qlt6dWDCSUG55v9?e=ZJcHsV</t>
+  </si>
+  <si>
+    <t>Automated essay scoring</t>
+  </si>
+  <si>
+    <t>RQ1 What are the datasets available for research on automated essay grading?|RQ2 What are the features extracted for the assessment of essays?|RQ3 Which  are  the  evaluation  metrics  available  for  measuring  the  accuracy  of  algorithms?|RQ4 What are the Machine Learning techniques used for automatic essay grading, and how are they implemented?|RQ5 What are the challenges/limitations in the current research?</t>
+  </si>
+  <si>
+    <t>PICOC</t>
+  </si>
+  <si>
+    <t>ACL, ACM, IEEE Explore, Springer, Science Direct</t>
+  </si>
+  <si>
+    <t>search_string</t>
+  </si>
+  <si>
+    <t>“Automated essay grading” OR “Automated essay scoring” OR “short answer scoring systems” OR “essay scoring systems” OR “auto-matic essay evaluation”</t>
+  </si>
+  <si>
+    <t>IC1 Our approach is to work with datasets comprise of essays written in English. We excluded the essays written in other languages.|IC2 We included the papers implemented on the AI approach and excluded the traditional methods for the review.|IC3 The study is on essay scoring systems, so we exclusively included the research carried out on only text data sets rather than other datasets like image or speech.|EC1 We removed the papers in the form of review papers, survey papers, and state of the art papers.</t>
+  </si>
+  <si>
+    <t>QA1: Internal validity.|QA2: External validity.|QA3: Bias.</t>
+  </si>
+  <si>
+    <t>542|62</t>
+  </si>
+  <si>
+    <t>System|Approach|Dataset|Features applied|Evaluation metric and results|Cohesion|Coherence|Completeness|Feed Back|Grammar|Style|Mechanics|Development|BoW|Relevance</t>
+  </si>
+  <si>
+    <t>Multi-object tracking in traffic environments</t>
+  </si>
+  <si>
+    <t>IEEE Xplore|Web of Science|Springer-Link|ACM Digital Library|Scopus</t>
+  </si>
+  <si>
+    <t>RQ1 Which are the main techniques for Multi-Object Tracing in traffic environments?|RQ2 Which are the devices used for Multi-Object Tracing in traffic environments?|RQ3 Which are the main datasets for Multi-Object Tracing in traffic environments?|RQ4 Which are the evaluation metrics for Multi-Object Tracing in traffic environments?|RQ5 What are the main open lines of research or issues in this domain?</t>
+  </si>
+  <si>
+    <t>800|35</t>
+  </si>
+  <si>
+    <t>Deep learning for mobile malware detection</t>
+  </si>
+  <si>
+    <t>RQ1 Which machine learning categories (supervised/unsupervised/semi-supervised/reinforcement learning) have been prefered in deep learning-based mobile malware detection?|RQ2 What data sources/features (e.g., API calls and system calls) have been used for the development of the malware detection models?|RQ3 What kind of deep learning algorithms (e.g., CNN and LSTM) have been applied?|RQ4 What kind of evaluation parameters (e.g., accuracy) and evaluation approaches (e.g., cross-validation) has been used?|RQ5 Which deep learning algorithm works best for mobile malware detection?|RQ6 What kind of feature selection techniques have been used?|RQ7 Which public datasets have been analyzed during the development of the model?|RQ8 Which deep learning platforms have been used for the implementation of the models??|RQ9 what are the challenges and research gaps in mobile malware detection?</t>
+  </si>
+  <si>
+    <t>ACM, IEEE Xplore, ScienceDirect, Springer, Wiley</t>
+  </si>
+  <si>
+    <t>"multi-object tracking OR "multi object tracking" OR "MOT" OR "multi-target tracking" OR "multi target tracking" OR "traffic" OR "urban" OR "environment" OR "vehicle" OR "city" OR "road" OR "lane" OR "motorway"</t>
+  </si>
+  <si>
+    <t>"deep learning AND ("malware detection" OR "malware classification" OR "malware analysis")</t>
+  </si>
+  <si>
+    <t>Figure 1</t>
+  </si>
+  <si>
+    <t>1725|40</t>
+  </si>
+  <si>
+    <t>EC1 Duplicate papers form multiple sources.|EC2 Papers without full text available.|EC3 Papers not written in English.|EC4 Papers not published in a journal.|EC5 Short papers, editorials, issue introduction.|EC6 Secondary studies, such as literature review, SMS, SLR.|EC7 Papers which do not use deep learning to detect malware in mobile application.|EC8 Papers which only use traditional ML algorithms.|EC9 Papers which do not include empirical results.</t>
+  </si>
+  <si>
+    <t>QA1 Are the aims of the study clearly stated?|QA2 Are the scope and context and experimental design of the study clearly defined?|QA3 Are the variables in the study likely to be valid and reliable?|QA4 Is the research proces documented adequately?|QA5 Are all the study questions answered?|QA6 Are the negative findings presented?|QA7 Are the main findings stated clearly (regarding credibility, validity, and reliability)?|QA8 Do the conclusions relate to the aim of the purpose of the study, and are they reliable?</t>
+  </si>
+  <si>
+    <t>Journal title|Publication year|Paper title|Abstract|ML category|Type of analysis|Data sources|DL approaches|Evaluation parameters|Validation method|Best algorithm|Feature selection method|Evaluation dataset|Implementation platform|Cahllenges and proposed solutions</t>
+  </si>
+  <si>
+    <t>Deep learning for process prediction</t>
+  </si>
+  <si>
+    <t>RQ1 Which kind of neural network is used for prediction?|RQ2 Which pre-processing steps are carried out?|RQ3 How it the data being encoded?|RQ4 What is the prediction target?|RQ5 Are there dominant approaches or does every approach come with its own advantages?|RQ6 Are the proposed approaches combinable?</t>
+  </si>
+  <si>
+    <t>Web of Science, Science Direct, IEEE Explore, ACM Digital Library, SpringerLink</t>
+  </si>
+  <si>
+    <t>(((“All Metadata”:“Business process*”) AND “All Meta-data”:Predicti*) AND “All Metadata”:“Deep Learning”)|(((“All Metadata”:“Business process*”) AND “All Meta-data”:Predicti*) AND “All Metadata”:“*Neural Networks*”)</t>
+  </si>
+  <si>
+    <t>Database (IEEE Xplore) specific search strings</t>
+  </si>
+  <si>
+    <t>IN1 The study is related to business process prediction and reports an implemented and evaluated approach.|IN2 The study uses a deep learning method, i.e. some form of neural network for predic-tion or it combines traditional machine learning algorithms with a deep learning architecture.|EX1 The study is not published in English.|EX2 The study is not freely accessible through the standard university libraries proxy services or it is electronically unavailable.|EX3 The study or the presented approach is not related to the field of computer science.</t>
+  </si>
+  <si>
+    <t>144|32</t>
+  </si>
+  <si>
+    <t>Study|Type|Target|Input|Encoding</t>
+  </si>
+  <si>
+    <t>Machine learning in mechanical fault diagnosis and prognosis</t>
+  </si>
+  <si>
+    <t>PRISMA adopted</t>
+  </si>
+  <si>
+    <t>RQ1 In which publication venues are studies about the use of machine learning for mechanical fault detection and fault prognosis in manufacturing equipment published?|RQ2 In which scientific fields has the use of machine learning for mechanical fault detection and fault prognosis in manufacturing equipment been researched?|RQ3 What machine learning algorithms and methods are currently employed for mechanical fault detection and fault prognosis in manufacturing equipment?|RQ4 What limitations and advantages do those algorithms and methods present?|RQ5 Which of those algorithms and methods are used for data stream learning?</t>
+  </si>
+  <si>
+    <t>Web of Science, ACM Digital Library, Science Direct, Wiley Online Library, IEEE Xplore</t>
+  </si>
+  <si>
+    <t>IC1 The publication focuses on the use of machine learning algorithms and methods for mechanical fault detection in manufacturing equipment.|IC2 The publication focuses on the use of machine learning algorithms and methods for prognosis of faults in manufacturing equipment.|EC1 Duplicate publication.|EC2 Publication is not a full-length article.|EC3 Study not published in a peer-reviewd journal with JCR Impact Factor, in conference proceedings, or in a book chapter/section.|EC4 Study published befor 2015.|EC5 Publication not written in English.|EC6 Study without empirical results obtained from an industrial case-study.</t>
+  </si>
+  <si>
+    <t>(("mining" OR "learning" OR "knowledge discovery") AND ("fault detection" OR "fault prediction" OR "fault prognosis" OR "predictive maintenance"))</t>
+  </si>
+  <si>
+    <t>4549|44</t>
+  </si>
+  <si>
+    <t>Title|Authors|Country of research|Publication venue|Publication details|Type of publication venue|Scientific field|Research questions answered|Machine learning method|Learning task</t>
+  </si>
+  <si>
+    <t>Software security management in critical infrastructures</t>
+  </si>
+  <si>
+    <t>RQ1 What are the identified software security threats in CIs?|RQ2 What are the proposed solution for coping with the software security threats in CIs?|RQ3 Which CI domains have been identified related to software security?|RQ4 What are the adopted evaluation approaches of CIs with respect to software security?</t>
+  </si>
+  <si>
+    <t>ACM Digital Library, IEEE Xplore, Science Direct, Wiley Online Library</t>
+  </si>
+  <si>
+    <t>("Document Title":security management) AND ("Full Text Only":data intensive systems) AND ("Full Text Only":critical infrastructures) AND ("All Metadata":software) Filters Applied: 2010 - 2021</t>
+  </si>
+  <si>
+    <t>EC1 Paper where the full text is not available.|EC2 Paper does not relate to software engineering.|EC3 Paper does not relate to software security management.|EC4 Paper does not relate ot critical infrastructures.|EC5 Paper does not satisfy the scope of this research.|EC6 Duplicate publications found in different search sources.|EC7 Papers that are experience, proposal, critical review, and survey papers.</t>
+  </si>
+  <si>
+    <t>1087|32</t>
+  </si>
+  <si>
+    <t>QA1 Are the main theme and motivation of the study clearly stated?|QA2 Do the researchers clearly define the scope and context of the study?|QA3 Do the researchers clearly define methods/approaches/technologies given in the study?|QA4 Do the researches clearly explain the proposed solution and validate them by an empirical study?|QA5 Is the study reporting clear and coherent?|QA6 Do the researches answer all the study questions?|QA7 Do the researchers present negative findings in the study?|QA8 Do the  researchers explain the consequences of any problems with the validity/reliability of their measures?|QA9 Do the conclusions satisfy the purpose of the study?|QA10 Does the study have implications in practice and results in a research area for software security management in critical infrastructures?</t>
+  </si>
+  <si>
+    <t>ID|Title|Year|Authors|Repository|Publication type|Publication channel|Keywords|Main theme of study|Motivation for study|Security management methodology/technology/technique/type|Contribution type|CI domain|Solution area|Assessment approach|Evidence type|Findings|Constraints, limitations and chalenges of proposed solution</t>
+  </si>
+  <si>
+    <t>Spam content detection and classification</t>
+  </si>
+  <si>
+    <t>Web of Science, Scopus, Springer, IEEE Xplore, ACM Digial Library, Science Direct</t>
+  </si>
+  <si>
+    <t>social spam|spam AND Twitter|spam AND artificial intelligence|social spam AND artificial intelligence|online spam AND review spam|social media AND spam</t>
+  </si>
+  <si>
+    <t>Study|Dataset|Classification approach|Merits|Limitations|Results</t>
+  </si>
+  <si>
+    <t>Current approaches for executing big data science projects</t>
+  </si>
+  <si>
+    <t>RQ1 Has research in this domain increased recently?|RQ2 What are the most common approaches regarding how data science projects are organized, managed and coordinated?|RQ3: What are the phases or activities in a data science project life cycle?</t>
+  </si>
+  <si>
+    <t>ACM Digital Library, IEEEXplore, Scopus, Science Direct, Google Scholar</t>
+  </si>
+  <si>
+    <t>IC1 Papers that fully or partly include a description of the organization, management or coordination of big data science projects.|IC2 Papers that suggest specific approaches for executing big data science projects.|IC3 Papers that were published after 2015. EC1 Papers that are not written in English.|EC2 Papers that did not focus on data science team process, but rather, focused on using data analytics to improve overall project management processes were excluded.|EC3 Papers that had no form of peer review (e.g. blogs).EC4 Papers with irrelevant document type such as posters, conference summaries, etc.</t>
+  </si>
+  <si>
+    <t>(“data science” OR “big data” OR “machine learning”) AND (“process methodology” OR “team process” OR “teamcoordination” OR “project management”)</t>
+  </si>
+  <si>
+    <t>2450|68</t>
   </si>
 </sst>
 </file>
@@ -803,11 +974,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,9 +986,19 @@
     <col min="5" max="5" width="33.85546875" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" customWidth="1"/>
+    <col min="15" max="15" width="27.42578125" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,30 +1036,33 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -890,31 +1074,48 @@
         <v>19</v>
       </c>
       <c r="F2">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
+      <c r="Q2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -923,34 +1124,42 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3">
         <v>2022</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+        <v>70</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
+      <c r="Q3" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -959,34 +1168,54 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4">
         <v>2022</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>88</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -995,34 +1224,47 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>2021</v>
+      </c>
+      <c r="G5" t="s">
         <v>26</v>
       </c>
-      <c r="F5">
-        <v>2022</v>
-      </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
       <c r="H5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
+      <c r="Q5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -1031,31 +1273,49 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6">
+        <v>2022</v>
+      </c>
+      <c r="G6" t="s">
         <v>28</v>
       </c>
-      <c r="G6" t="s">
-        <v>29</v>
-      </c>
       <c r="H6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
+      <c r="P6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7">
         <v>12</v>
@@ -1064,34 +1324,51 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7">
         <v>2022</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I7" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="P7" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8">
         <v>14</v>
@@ -1100,34 +1377,41 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8">
         <v>2022</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I8" t="s">
-        <v>21</v>
+        <v>108</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
+      <c r="L8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
+      <c r="R8" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9">
         <v>17</v>
@@ -1136,34 +1420,47 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9">
         <v>2022</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
+      <c r="K9" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
+      <c r="P9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10">
         <v>19</v>
@@ -1172,16 +1469,13 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
         <v>36</v>
       </c>
-      <c r="G10" t="s">
-        <v>37</v>
-      </c>
       <c r="H10" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -1193,10 +1487,11 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11">
         <v>20</v>
@@ -1205,19 +1500,16 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11">
         <v>2022</v>
       </c>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H11" t="s">
-        <v>57</v>
-      </c>
-      <c r="I11" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -1229,10 +1521,11 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12">
         <v>21</v>
@@ -1241,19 +1534,16 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12">
         <v>2022</v>
       </c>
       <c r="G12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H12" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1265,10 +1555,11 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13">
         <v>23</v>
@@ -1277,19 +1568,16 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F13">
         <v>2022</v>
       </c>
       <c r="G13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H13" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -1301,10 +1589,11 @@
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14">
         <v>24</v>
@@ -1313,19 +1602,16 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F14">
         <v>2022</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H14" t="s">
-        <v>60</v>
-      </c>
-      <c r="I14" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1337,6 +1623,7 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>